<commit_message>
Added time-based color code and filter by ID. Just PDF left.
</commit_message>
<xml_diff>
--- a/server/public/icbs_primax_test.xlsx
+++ b/server/public/icbs_primax_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Month</t>
   </si>
@@ -44,6 +44,9 @@
     <t>January</t>
   </si>
   <si>
+    <t>1/1/2023</t>
+  </si>
+  <si>
     <t>Sunday</t>
   </si>
   <si>
@@ -53,9 +56,18 @@
     <t>Marketing</t>
   </si>
   <si>
+    <t>5:00</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
     <t>February</t>
   </si>
   <si>
+    <t>1/2/2023</t>
+  </si>
+  <si>
     <t>Wednesday</t>
   </si>
   <si>
@@ -65,22 +77,34 @@
     <t>IT</t>
   </si>
   <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
     <t>March</t>
   </si>
   <si>
+    <t>1/3/2023</t>
+  </si>
+  <si>
     <t>Leather Face</t>
   </si>
   <si>
     <t>Hacker</t>
+  </si>
+  <si>
+    <t>9:00</t>
+  </si>
+  <si>
+    <t>17:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -108,17 +132,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -373,26 +394,26 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>44927.0</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.5416666666666666</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I2" s="1">
         <v>8.0</v>
@@ -400,28 +421,28 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44928.0</v>
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
         <v>2.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.2916666666666667</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.625</v>
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="I3" s="1">
         <v>8.0</v>
@@ -429,28 +450,28 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44929.0</v>
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>3.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.7083333333333334</v>
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="I4" s="1">
         <v>8.0</v>

</xml_diff>